<commit_message>
Ejercicio 3 de Base de Datos
</commit_message>
<xml_diff>
--- a/Avance 1/Requisitos.xlsx
+++ b/Avance 1/Requisitos.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="47">
   <si>
     <t>Requisito</t>
   </si>
@@ -146,6 +146,12 @@
   </si>
   <si>
     <t>Cargar imagen</t>
+  </si>
+  <si>
+    <t>Generar reportes</t>
+  </si>
+  <si>
+    <t>Consultar reportes</t>
   </si>
 </sst>
 </file>
@@ -837,12 +843,34 @@
       <c r="H37" s="8"/>
     </row>
     <row r="38">
-      <c r="B38" s="1"/>
-      <c r="D38" s="1"/>
+      <c r="B38" s="9">
+        <v>11.0</v>
+      </c>
+      <c r="C38" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="D38" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="E38" s="8"/>
+      <c r="F38" s="8"/>
+      <c r="G38" s="8"/>
+      <c r="H38" s="8"/>
     </row>
     <row r="39">
-      <c r="B39" s="1"/>
-      <c r="D39" s="1"/>
+      <c r="B39" s="9">
+        <v>11.1</v>
+      </c>
+      <c r="C39" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D39" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="E39" s="8"/>
+      <c r="F39" s="8"/>
+      <c r="G39" s="8"/>
+      <c r="H39" s="8"/>
     </row>
     <row r="40">
       <c r="B40" s="1"/>

</xml_diff>